<commit_message>
Upload Y3_B2526_CNS_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y3_B2526_CNS_schedule.xlsx
+++ b/modules_schedules/Y3_B2526_CNS_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BDFBB3-47CC-475D-92C7-B5E101F160E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC23B3D-107A-48F1-A621-5A0B31A533A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CNS" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>16/11/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">biochemistry </t>
-  </si>
-  <si>
     <t>histology</t>
   </si>
   <si>
@@ -119,6 +116,9 @@
   </si>
   <si>
     <t>25/09/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biochemistry Lab/CBL </t>
   </si>
 </sst>
 </file>
@@ -760,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -783,13 +783,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
@@ -806,16 +806,16 @@
         <v>8</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="6">
         <v>2</v>
       </c>
       <c r="E13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="G13" s="9">
         <v>120</v>
@@ -829,13 +829,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2">
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>16</v>
@@ -852,7 +852,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="6">
         <v>4</v>
@@ -861,7 +861,7 @@
         <v>45970</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G15" s="9">
         <v>120</v>
@@ -875,13 +875,13 @@
         <v>8</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D16" s="2">
         <v>1</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>12</v>
@@ -898,13 +898,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="6">
         <v>2</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>12</v>
@@ -921,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2">
         <v>3</v>
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -967,13 +967,13 @@
         <v>8</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2">
         <v>2</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" s="4">
         <v>0.41666666666666669</v>
@@ -990,13 +990,13 @@
         <v>8</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="6">
         <v>2</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>12</v>
@@ -1013,7 +1013,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2">
         <v>3</v>
@@ -1036,7 +1036,7 @@
         <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="6">
         <v>4</v>
@@ -1056,7 +1056,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>9</v>
@@ -1065,7 +1065,7 @@
         <v>10</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>16</v>
@@ -1079,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>9</v>
@@ -1102,7 +1102,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>9</v>
@@ -1125,7 +1125,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>9</v>
@@ -1137,7 +1137,7 @@
         <v>14</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G27" s="9">
         <v>120</v>
@@ -1148,7 +1148,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>9</v>
@@ -1171,7 +1171,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>9</v>
@@ -1194,7 +1194,7 @@
         <v>7</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -1217,7 +1217,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>9</v>
@@ -1240,7 +1240,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>9</v>
@@ -1252,7 +1252,7 @@
         <v>19</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32" s="5">
         <v>120</v>
@@ -1263,10 +1263,10 @@
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D33" s="6">
         <v>1</v>
@@ -1286,19 +1286,19 @@
         <v>7</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G34" s="5">
         <v>120</v>
@@ -1309,16 +1309,16 @@
         <v>7</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D35" s="6">
         <v>2</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>12</v>
@@ -1332,16 +1332,16 @@
         <v>7</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2">
         <v>3</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" s="4">
         <v>0.58333333333333337</v>
@@ -1355,10 +1355,10 @@
         <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" s="6">
         <v>4</v>
@@ -1378,19 +1378,19 @@
         <v>7</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" s="2">
         <v>1</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="G38" s="5">
         <v>120</v>
@@ -1401,19 +1401,19 @@
         <v>7</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" s="6">
         <v>2</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G39" s="9">
         <v>120</v>
@@ -1424,10 +1424,10 @@
         <v>7</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D40" s="2">
         <v>3</v>
@@ -1447,10 +1447,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="6">
         <v>1</v>
@@ -1459,7 +1459,7 @@
         <v>45936</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G41" s="9">
         <v>120</v>
@@ -1470,19 +1470,19 @@
         <v>7</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G42" s="5">
         <v>120</v>
@@ -1493,19 +1493,19 @@
         <v>7</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="6">
         <v>2</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G43" s="9">
         <v>120</v>
@@ -1516,10 +1516,10 @@
         <v>7</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="2">
         <v>3</v>
@@ -1528,7 +1528,7 @@
         <v>45965</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G44" s="5">
         <v>120</v>
@@ -1539,10 +1539,10 @@
         <v>7</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="6">
         <v>4</v>
@@ -1551,7 +1551,7 @@
         <v>45970</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G45" s="9">
         <v>120</v>

</xml_diff>